<commit_message>
Make TreeSim a variable for altering simplification steps
</commit_message>
<xml_diff>
--- a/src/TreeSeqCompTime.xlsx
+++ b/src/TreeSeqCompTime.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="15780" tabRatio="500"/>
+    <workbookView xWindow="4040" yWindow="540" windowWidth="24360" windowHeight="8760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,19 +27,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>TreeSeqSimp</t>
   </si>
   <si>
     <t>CPU</t>
   </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>Peak Memory_GB</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -51,6 +57,21 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Menlo"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Menlo Regular"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo Regular"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Menlo Regular"/>
     </font>
   </fonts>
   <fills count="2">
@@ -73,9 +94,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -353,65 +393,185 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" customWidth="1"/>
+    <col min="4" max="4" width="17" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="7"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="7">
+        <v>25</v>
+      </c>
+      <c r="B2" s="1">
+        <v>26024.2</v>
+      </c>
+      <c r="C2" s="9">
+        <f>B2/3600</f>
+        <v>7.2289444444444451</v>
+      </c>
+      <c r="D2" s="1">
+        <v>10.143000000000001</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="7">
+        <v>50</v>
+      </c>
+      <c r="B3" s="1">
+        <v>20554.7</v>
+      </c>
+      <c r="C3" s="9">
+        <f>B3/3600</f>
+        <v>5.7096388888888887</v>
+      </c>
+      <c r="D3" s="1">
+        <v>18.760000000000002</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="7">
         <v>100</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B4" s="4">
         <v>19575.7</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="C4" s="9">
+        <f>B4/3600</f>
+        <v>5.4376944444444444</v>
+      </c>
+      <c r="D4" s="4">
+        <v>35.820999999999998</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="7">
         <v>250</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B5" s="4">
         <v>21464.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="C5" s="9">
+        <f>B5/3600</f>
+        <v>5.962361111111111</v>
+      </c>
+      <c r="D5" s="5">
+        <v>87.296999999999997</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="7">
         <v>500</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="B6" s="7">
+        <v>21371</v>
+      </c>
+      <c r="C6" s="9">
+        <f>B6/3600</f>
+        <v>5.9363888888888887</v>
+      </c>
+      <c r="D6" s="5">
+        <v>173.13399999999999</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="7">
         <v>750</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="B7" s="7"/>
+      <c r="C7" s="9">
+        <f t="shared" ref="C6:C10" si="0">B7/3600</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="7">
         <v>1000</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="B8" s="7"/>
+      <c r="C8" s="9">
+        <v>0</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="7">
         <v>2000</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="B9" s="7"/>
+      <c r="C9" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="7">
         <v>3000</v>
       </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add CompTime and MemUsage Figure & update parameter space
</commit_message>
<xml_diff>
--- a/src/TreeSeqCompTime.xlsx
+++ b/src/TreeSeqCompTime.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4040" yWindow="540" windowWidth="24360" windowHeight="8760" tabRatio="500"/>
+    <workbookView xWindow="13240" yWindow="540" windowWidth="14300" windowHeight="8760" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TreeSeqCompTime.csv" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -94,7 +94,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -114,6 +114,9 @@
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -393,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -423,155 +426,189 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1">
-        <v>26024.2</v>
+        <v>33315.4</v>
       </c>
       <c r="C2" s="9">
         <f>B2/3600</f>
-        <v>7.2289444444444451</v>
-      </c>
-      <c r="D2" s="1">
-        <v>10.143000000000001</v>
+        <v>9.2542777777777783</v>
+      </c>
+      <c r="D2" s="10">
+        <v>7.3789999999999996</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1">
-        <v>20554.7</v>
+        <v>30716.6</v>
       </c>
       <c r="C3" s="9">
-        <f>B3/3600</f>
-        <v>5.7096388888888887</v>
-      </c>
-      <c r="D3" s="1">
-        <v>18.760000000000002</v>
+        <f t="shared" ref="C3:C7" si="0">B3/3600</f>
+        <v>8.5323888888888888</v>
+      </c>
+      <c r="D3" s="10">
+        <v>9.3859999999999992</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
-        <v>100</v>
-      </c>
-      <c r="B4" s="4">
-        <v>19575.7</v>
+        <v>25</v>
+      </c>
+      <c r="B4" s="1">
+        <v>26024.2</v>
       </c>
       <c r="C4" s="9">
-        <f>B4/3600</f>
-        <v>5.4376944444444444</v>
-      </c>
-      <c r="D4" s="4">
-        <v>35.820999999999998</v>
+        <f t="shared" si="0"/>
+        <v>7.2289444444444451</v>
+      </c>
+      <c r="D4" s="11">
+        <v>10.143000000000001</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
-        <v>250</v>
-      </c>
-      <c r="B5" s="4">
-        <v>21464.5</v>
+        <v>30</v>
+      </c>
+      <c r="B5" s="1">
+        <v>26777.8</v>
       </c>
       <c r="C5" s="9">
-        <f>B5/3600</f>
-        <v>5.962361111111111</v>
-      </c>
-      <c r="D5" s="5">
-        <v>87.296999999999997</v>
+        <f t="shared" si="0"/>
+        <v>7.4382777777777775</v>
+      </c>
+      <c r="D5" s="11">
+        <v>12.818</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
-        <v>500</v>
-      </c>
-      <c r="B6" s="7">
-        <v>21371</v>
+        <v>35</v>
+      </c>
+      <c r="B6" s="1">
+        <v>24486</v>
       </c>
       <c r="C6" s="9">
-        <f>B6/3600</f>
-        <v>5.9363888888888887</v>
-      </c>
-      <c r="D6" s="5">
-        <v>173.13399999999999</v>
+        <f t="shared" si="0"/>
+        <v>6.8016666666666667</v>
+      </c>
+      <c r="D6" s="11">
+        <v>13.61</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
-        <v>750</v>
-      </c>
-      <c r="B7" s="7"/>
+        <v>40</v>
+      </c>
+      <c r="B7" s="1">
+        <v>23265.3</v>
+      </c>
       <c r="C7" s="9">
-        <f t="shared" ref="C6:C10" si="0">B7/3600</f>
-        <v>0</v>
-      </c>
-      <c r="D7" s="10"/>
+        <f t="shared" si="0"/>
+        <v>6.4625833333333329</v>
+      </c>
+      <c r="D7" s="11">
+        <v>15.286</v>
+      </c>
       <c r="E7" s="7"/>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
-        <v>1000</v>
-      </c>
-      <c r="B8" s="7"/>
+        <v>50</v>
+      </c>
+      <c r="B8" s="1">
+        <v>20554.7</v>
+      </c>
       <c r="C8" s="9">
-        <v>0</v>
-      </c>
-      <c r="D8" s="10"/>
+        <f>B8/3600</f>
+        <v>5.7096388888888887</v>
+      </c>
+      <c r="D8" s="11">
+        <v>18.760000000000002</v>
+      </c>
       <c r="E8" s="7"/>
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
-        <v>2000</v>
-      </c>
-      <c r="B9" s="7"/>
+        <v>100</v>
+      </c>
+      <c r="B9" s="4">
+        <v>19575.7</v>
+      </c>
       <c r="C9" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D9" s="10"/>
+        <f>B9/3600</f>
+        <v>5.4376944444444444</v>
+      </c>
+      <c r="D9" s="5">
+        <v>35.820999999999998</v>
+      </c>
       <c r="E9" s="7"/>
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
-        <v>3000</v>
-      </c>
-      <c r="B10" s="7"/>
+        <v>250</v>
+      </c>
+      <c r="B10" s="4">
+        <v>21464.5</v>
+      </c>
       <c r="C10" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D10" s="10"/>
+        <f>B10/3600</f>
+        <v>5.962361111111111</v>
+      </c>
+      <c r="D10" s="5">
+        <v>87.296999999999997</v>
+      </c>
       <c r="E10" s="7"/>
       <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="10"/>
+      <c r="A11" s="7">
+        <v>500</v>
+      </c>
+      <c r="B11" s="7">
+        <v>21371</v>
+      </c>
+      <c r="C11" s="9">
+        <f>B11/3600</f>
+        <v>5.9363888888888887</v>
+      </c>
+      <c r="D11" s="5">
+        <v>173.13399999999999</v>
+      </c>
       <c r="E11" s="7"/>
       <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="3"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="7"/>
       <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Post Ben Meeting & Sara Overhaul of Outputs
</commit_message>
<xml_diff>
--- a/src/TreeSeqCompTime.xlsx
+++ b/src/TreeSeqCompTime.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13240" yWindow="540" windowWidth="14300" windowHeight="8760" tabRatio="500"/>
+    <workbookView xWindow="13760" yWindow="1180" windowWidth="13240" windowHeight="15740" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="TreeSeqCompTime.csv" sheetId="1" r:id="rId1"/>
+    <sheet name="TreeSeqCompTime" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -45,7 +45,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -57,21 +57,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Menlo"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Menlo Regular"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Menlo Regular"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Menlo Regular"/>
     </font>
   </fonts>
   <fills count="2">
@@ -94,31 +79,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,219 +360,198 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="14.1640625" customWidth="1"/>
-    <col min="4" max="4" width="17" style="2" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="7">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1">
+        <v>51791.8</v>
+      </c>
+      <c r="C2" s="2">
+        <f>B2/3600</f>
+        <v>14.386611111111112</v>
+      </c>
+      <c r="D2">
+        <v>3.2469999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1">
+        <v>36732.699999999997</v>
+      </c>
+      <c r="C3" s="2">
+        <f>B3/3600</f>
+        <v>10.203527777777778</v>
+      </c>
+      <c r="D3">
+        <v>4.9610000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
         <v>15</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B4">
         <v>33315.4</v>
       </c>
-      <c r="C2" s="9">
-        <f>B2/3600</f>
+      <c r="C4" s="2">
+        <f>B4/3600</f>
         <v>9.2542777777777783</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D4">
         <v>7.3789999999999996</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="7">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>20</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B5">
         <v>30716.6</v>
       </c>
-      <c r="C3" s="9">
-        <f t="shared" ref="C3:C7" si="0">B3/3600</f>
-        <v>8.5323888888888888</v>
-      </c>
-      <c r="D3" s="10">
+      <c r="C5">
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="D5">
         <v>9.3859999999999992</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="7">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>25</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B6">
         <v>26024.2</v>
       </c>
-      <c r="C4" s="9">
-        <f t="shared" si="0"/>
-        <v>7.2289444444444451</v>
-      </c>
-      <c r="D4" s="11">
+      <c r="C6">
+        <v>7.23</v>
+      </c>
+      <c r="D6">
         <v>10.143000000000001</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="7">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>30</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B7">
         <v>26777.8</v>
       </c>
-      <c r="C5" s="9">
-        <f t="shared" si="0"/>
-        <v>7.4382777777777775</v>
-      </c>
-      <c r="D5" s="11">
+      <c r="C7">
+        <v>7.44</v>
+      </c>
+      <c r="D7">
         <v>12.818</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="7">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>35</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B8">
         <v>24486</v>
       </c>
-      <c r="C6" s="9">
-        <f t="shared" si="0"/>
-        <v>6.8016666666666667</v>
-      </c>
-      <c r="D6" s="11">
+      <c r="C8">
+        <v>6.8</v>
+      </c>
+      <c r="D8">
         <v>13.61</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="7">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
         <v>40</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B9">
         <v>23265.3</v>
       </c>
-      <c r="C7" s="9">
-        <f t="shared" si="0"/>
-        <v>6.4625833333333329</v>
-      </c>
-      <c r="D7" s="11">
+      <c r="C9">
+        <v>6.46</v>
+      </c>
+      <c r="D9">
         <v>15.286</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="7">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>50</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B10">
         <v>20554.7</v>
       </c>
-      <c r="C8" s="9">
-        <f>B8/3600</f>
-        <v>5.7096388888888887</v>
-      </c>
-      <c r="D8" s="11">
+      <c r="C10">
+        <v>5.71</v>
+      </c>
+      <c r="D10">
         <v>18.760000000000002</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="7">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>100</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B11">
         <v>19575.7</v>
       </c>
-      <c r="C9" s="9">
-        <f>B9/3600</f>
-        <v>5.4376944444444444</v>
-      </c>
-      <c r="D9" s="5">
+      <c r="C11">
+        <v>5.44</v>
+      </c>
+      <c r="D11">
         <v>35.820999999999998</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="7">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
         <v>250</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B12">
         <v>21464.5</v>
       </c>
-      <c r="C10" s="9">
-        <f>B10/3600</f>
-        <v>5.962361111111111</v>
-      </c>
-      <c r="D10" s="5">
+      <c r="C12">
+        <v>5.96</v>
+      </c>
+      <c r="D12">
         <v>87.296999999999997</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="7">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
         <v>500</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B13">
         <v>21371</v>
       </c>
-      <c r="C11" s="9">
-        <f>B11/3600</f>
-        <v>5.9363888888888887</v>
-      </c>
-      <c r="D11" s="5">
+      <c r="C13">
+        <v>5.94</v>
+      </c>
+      <c r="D13">
         <v>173.13399999999999</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>